<commit_message>
[FIX] fixing all plots after adding exchange rates
</commit_message>
<xml_diff>
--- a/financial_data/gomspace.xlsx
+++ b/financial_data/gomspace.xlsx
@@ -64,7 +64,7 @@
     <t>Tax</t>
   </si>
   <si>
-    <t>Net loss</t>
+    <t>Net Loss</t>
   </si>
   <si>
     <t>Goodwill</t>
@@ -182,19 +182,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -241,16 +235,16 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>